<commit_message>
add protol for android and ios
</commit_message>
<xml_diff>
--- a/蓝牙模块手机相机按键协议.xlsx
+++ b/蓝牙模块手机相机按键协议.xlsx
@@ -5,14 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoliang\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.0.106\cht\work\project\bt_transmit_git\bt_transmit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Android" sheetId="1" r:id="rId1"/>
+    <sheet name="IOS" sheetId="2" r:id="rId2"/>
+    <sheet name="蓝牙模块控制协议" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
   <si>
     <t>拍照</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -137,14 +139,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>备注：蓝牙模块(CSI_DEV)通过连接手机，给手机发送键盘事件完成，具体键盘事件请参考USB HID keycode</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>蓝牙模块手机相机控制协议</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>0x58 /* entry */</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -157,11 +151,736 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>Ios keycode</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>0x21 /* Key4 */</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>0x72 /* fingerprint identify end */</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x69 /* 401 */</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x6F /* fingerprint finger up */</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x6E /* fingerprint up */</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>0x20 /* Key3 */</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x6E /* fingerprint up */</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝牙模块android手机相机按键定义</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝牙模块ios手机相机按键定义</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注：蓝牙模块(BT Shutter-KUN)通过连接手机，给手机发送键盘事件完成，具体键盘事件请参考USB HID keycode</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x20 /* Key3 */</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1E /* Key1 */</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1F /* Key2 */</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Volume+</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝牙模块与手机控制命令</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x72 /* fingerprint identify end */</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00,0xE9 /* volume+ */</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x28 /* entry */</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>entry</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>协议命令格式：</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>协议头</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>数据长度</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>命令</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>子命令</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>负载</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>校验和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(共计20字节)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>协议头</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>一般由0xAA或0x55构成，0xAA表示该数据段有子命令，0x55则相反，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>占用1字节</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>；</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>数据长度</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>表示负载有效数据的长度，多余数据位则为0，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>占用1字节</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>；</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>命令</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>为蓝牙主命令，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>占用1字节</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>；</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>子命令</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>为蓝牙主命令的附属命令，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>占用1字节</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>；</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>负载</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>用来传递有效数据，与数据长度对应，一般</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>占用15字节</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>组成；</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>校验和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>用来校验整条数据的累计和是否等于0，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>占用1字节</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>；</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>命令</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统类型</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于蓝牙模块获取Master端系统类型</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据长度</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>命令</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>子命令</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>负载</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>检验和</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>协议头</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x55</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x04</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01:ios/0x02:android/0x03:windowsphone</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>参考校验和计算</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>按键方式</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>用选择蓝牙模块按键长按是否有效</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x02</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01:长按无效/0x00:长按有效</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Service UUID：0000fff0-0000-1000-8000-00805f9b34fb</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>primary service</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Characteristic UUID：0000fff2-0000-1000-8000-00805f9b34fb</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Properties：WRITE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝牙协议通信服务地址</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>校验和计算：</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -169,7 +888,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,8 +960,60 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,8 +1049,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -535,8 +1311,206 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -547,13 +1521,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -562,6 +1536,53 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -583,7 +1604,13 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -607,14 +1634,132 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="40% - 着色 5" xfId="2" builtinId="47"/>
     <cellStyle name="60% - 着色 5" xfId="3" builtinId="48"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="着色 2" xfId="4" builtinId="33"/>
     <cellStyle name="着色 5" xfId="1" builtinId="45"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -628,6 +1773,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>20775</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>53295</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1" descr="屏幕剪辑"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6576391"/>
+          <a:ext cx="3458058" cy="2057687"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -896,297 +2090,1392 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:G8"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="1" max="1" width="8.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="11"/>
+      <c r="A1" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="27"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="14"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="15" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="8"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="6"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="33"/>
+      <c r="B5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="33"/>
+      <c r="B6" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="33"/>
+      <c r="B7" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="34"/>
+      <c r="B8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B9" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="43"/>
+      <c r="B12" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="43"/>
+      <c r="B13" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="43"/>
+      <c r="B14" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="44"/>
+      <c r="B15" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="19"/>
+      <c r="B17" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="19"/>
+      <c r="B18" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="19"/>
+      <c r="B19" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="35"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="37"/>
+    </row>
+    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="40"/>
+    </row>
+    <row r="23" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="42">
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="A21:N21"/>
+    <mergeCell ref="A22:N22"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="H14:M14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="A1:N2"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="H7:M7"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="H20:M20"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="27"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="47"/>
       <c r="B5" s="24" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
       <c r="E5" s="24"/>
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="6"/>
+      <c r="H5" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>2</v>
+      <c r="A6" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="6"/>
+      <c r="H6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>3</v>
+      <c r="A7" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="6"/>
+      <c r="H7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="46"/>
+      <c r="B9" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="46"/>
+      <c r="B10" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="46"/>
+      <c r="B11" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="47"/>
+      <c r="B12" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B13" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="52"/>
+      <c r="B14" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="52"/>
+      <c r="B15" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="19"/>
-    </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="22"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="52"/>
+      <c r="B16" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="53"/>
+      <c r="B17" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="35"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="37"/>
+    </row>
+    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="28">
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="A1:N2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="H7:M7"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="A9:N9"/>
-    <mergeCell ref="A10:N10"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="H8:M12"/>
+    <mergeCell ref="H13:M17"/>
+    <mergeCell ref="A18:N18"/>
+    <mergeCell ref="A19:N19"/>
+    <mergeCell ref="A8:A12"/>
     <mergeCell ref="B8:G8"/>
-    <mergeCell ref="A1:N2"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="H4:M4"/>
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N30"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="27"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="74"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="76"/>
+    </row>
+    <row r="3" spans="1:14" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="79"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="80" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="81"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="68"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="65"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="65"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="65"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="64" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="65"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="65"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="65"/>
+    </row>
+    <row r="12" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="68"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="65"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="B14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="65"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="11"/>
+      <c r="B15" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="72"/>
+      <c r="L15" s="72"/>
+      <c r="M15" s="72"/>
+      <c r="N15" s="73"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="11"/>
+      <c r="B16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="72"/>
+      <c r="K16" s="72"/>
+      <c r="L16" s="72"/>
+      <c r="M16" s="72"/>
+      <c r="N16" s="73"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="11"/>
+      <c r="B17" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="65"/>
+    </row>
+    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="70"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A1:N2"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C17:N17"/>
+    <mergeCell ref="B12:N12"/>
+    <mergeCell ref="C18:N18"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="C13:N13"/>
+    <mergeCell ref="C14:N14"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="C16:N16"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>